<commit_message>
Added complete invoice generation and partial receipt generation
TODO: Different output formats, auto-match receipts etc.
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ydhanania\personal\finance\bulkinvoicer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5A416A-3913-43BB-A35A-C06650D31CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB1D60C-8D3F-4AED-8F63-5ACAF35410EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -127,20 +127,20 @@
     <t>Mr. Spencer Bradford</t>
   </si>
   <si>
-    <t>123, Golden Palance
+    <t>+91-1234567890</t>
+  </si>
+  <si>
+    <t>payment mode</t>
+  </si>
+  <si>
+    <t>cash</t>
+  </si>
+  <si>
+    <t>Advanced Tools</t>
+  </si>
+  <si>
+    <t>123, Golden Palace
 Kolkata, India</t>
-  </si>
-  <si>
-    <t>+91-1234567890</t>
-  </si>
-  <si>
-    <t>payment mode</t>
-  </si>
-  <si>
-    <t>cash</t>
-  </si>
-  <si>
-    <t>Advanced Tools</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F65D18-D01D-4049-B5EA-2A1952738832}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -506,10 +508,10 @@
         <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -749,7 +751,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7">
         <v>1000</v>
@@ -802,7 +804,7 @@
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -819,7 +821,7 @@
         <v>500</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
@@ -836,7 +838,7 @@
         <v>600</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding auto-match for invoices and receipts
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29204"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ydhanania\personal\finance\bulkinvoicer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB1D60C-8D3F-4AED-8F63-5ACAF35410EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF555C8-C5E9-48B4-B684-23D4F2940E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13749" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>name</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>payment mode</t>
-  </si>
-  <si>
-    <t>cash</t>
   </si>
   <si>
     <t>Advanced Tools</t>
@@ -141,6 +138,21 @@
   <si>
     <t>123, Golden Palace
 Kolkata, India</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>UPI</t>
+  </si>
+  <si>
+    <t>abc123</t>
+  </si>
+  <si>
+    <t>REC-2025-003</t>
+  </si>
+  <si>
+    <t>Cash</t>
   </si>
 </sst>
 </file>
@@ -471,7 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F65D18-D01D-4049-B5EA-2A1952738832}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -508,7 +520,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>29</v>
@@ -751,7 +763,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7">
         <v>1000</v>
@@ -780,9 +792,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B98120E-995E-44ED-82A5-A8C23CB48EE2}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -790,7 +804,7 @@
     <col min="2" max="2" width="10.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -806,8 +820,11 @@
       <c r="E1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -821,10 +838,10 @@
         <v>500</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -835,10 +852,30 @@
         <v>18</v>
       </c>
       <c r="D3">
-        <v>600</v>
+        <v>2600</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45905</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>700</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Font and cover page changes
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ydhanania\personal\finance\bulkinvoicer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF555C8-C5E9-48B4-B684-23D4F2940E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FE5EA0-4163-4DFE-967D-3BF140EFBA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13749" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>name</t>
   </si>
@@ -153,6 +153,51 @@
   </si>
   <si>
     <t>Cash</t>
+  </si>
+  <si>
+    <t>REC-2025-004</t>
+  </si>
+  <si>
+    <t>REC-2025-005</t>
+  </si>
+  <si>
+    <t>REC-2025-006</t>
+  </si>
+  <si>
+    <t>REC-2025-007</t>
+  </si>
+  <si>
+    <t>REC-2025-008</t>
+  </si>
+  <si>
+    <t>REC-2025-009</t>
+  </si>
+  <si>
+    <t>REC-2025-010</t>
+  </si>
+  <si>
+    <t>REC-2025-011</t>
+  </si>
+  <si>
+    <t>REC-2025-012</t>
+  </si>
+  <si>
+    <t>REC-2025-013</t>
+  </si>
+  <si>
+    <t>REC-2025-014</t>
+  </si>
+  <si>
+    <t>REC-2025-015</t>
+  </si>
+  <si>
+    <t>REC-2025-016</t>
+  </si>
+  <si>
+    <t>REC-2025-017</t>
+  </si>
+  <si>
+    <t>REC-2025-018</t>
   </si>
 </sst>
 </file>
@@ -792,10 +837,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B98120E-995E-44ED-82A5-A8C23CB48EE2}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -878,6 +923,81 @@
         <v>37</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>